<commit_message>
fix cycling in clean
</commit_message>
<xml_diff>
--- a/tests/simple.xlsx
+++ b/tests/simple.xlsx
@@ -30,6 +30,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -190,13 +191,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -208,6 +209,12 @@
       <c r="C1" s="1" t="e">
         <f aca="false">selectif(2,A1=1,A1+B1,)</f>
         <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <f aca="false">A1+B1</f>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add all vars some fixes
</commit_message>
<xml_diff>
--- a/tests/simple.xlsx
+++ b/tests/simple.xlsx
@@ -194,10 +194,10 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -215,6 +215,10 @@
       <c r="A2" s="0" t="n">
         <f aca="false">A1+B1</f>
         <v>3</v>
+      </c>
+      <c r="C2" s="0" t="e">
+        <f aca="false">selectif(2,A1=1,A2+B1,)</f>
+        <v>#NAME?</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
set 0 for novalue cells
</commit_message>
<xml_diff>
--- a/tests/simple.xlsx
+++ b/tests/simple.xlsx
@@ -118,20 +118,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF006600"/>
-        <sz val="10"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <name val="Arial"/>
@@ -251,19 +238,14 @@
         <v>#NAME?</v>
       </c>
       <c r="F2" s="2" t="e">
-        <f aca="false">selectif(0,E2&gt;1,E2+2,)</f>
+        <f aca="false">selectif(1,E2&gt;1,E2-2,)</f>
         <v>#NAME?</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1">
-    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>5</formula>
+    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>